<commit_message>
Agregada captura de periodicidad IVA
</commit_message>
<xml_diff>
--- a/dist/outputs/Iva-Estructurado.xlsx
+++ b/dist/outputs/Iva-Estructurado.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>Concepto</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>INVERSIONES ORTIZ VASQUEZ HERMANOS S A S</t>
+  </si>
+  <si>
+    <t>Periodicidad de la declaración</t>
+  </si>
+  <si>
+    <t>Cuatrimestral</t>
   </si>
   <si>
     <t>Ingresos por operaciones gravadas al 5%</t>
@@ -306,7 +312,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -355,10 +361,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>2019</v>
@@ -369,10 +375,10 @@
     </row>
     <row r="4" spans="1:5" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0</v>
@@ -386,10 +392,10 @@
     </row>
     <row r="5" spans="1:5" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>0</v>
@@ -403,10 +409,10 @@
     </row>
     <row r="6" spans="1:5" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>0</v>
@@ -420,10 +426,10 @@
     </row>
     <row r="7" spans="1:5" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>0</v>
@@ -437,10 +443,10 @@
     </row>
     <row r="8" spans="1:5" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0</v>
@@ -454,10 +460,10 @@
     </row>
     <row r="9" spans="1:5" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0</v>
@@ -471,10 +477,10 @@
     </row>
     <row r="10" spans="1:5" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0</v>
@@ -488,10 +494,10 @@
     </row>
     <row r="11" spans="1:5" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>0</v>
@@ -505,10 +511,10 @@
     </row>
     <row r="12" spans="1:5" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0</v>
@@ -522,10 +528,10 @@
     </row>
     <row r="13" spans="1:5" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0</v>
@@ -539,10 +545,10 @@
     </row>
     <row r="14" spans="1:5" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0</v>
@@ -556,13 +562,13 @@
     </row>
     <row r="15" spans="1:5" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>12688000</v>
+        <v>0</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>2019</v>
@@ -573,13 +579,13 @@
     </row>
     <row r="16" spans="1:5" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>9000</v>
+        <v>12688000</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>2019</v>
@@ -590,13 +596,13 @@
     </row>
     <row r="17" spans="1:5" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>12697000</v>
+        <v>9000</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>2019</v>
@@ -607,13 +613,13 @@
     </row>
     <row r="18" spans="1:5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>0</v>
+        <v>12697000</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>2019</v>
@@ -624,13 +630,13 @@
     </row>
     <row r="19" spans="1:5" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>12697000</v>
+        <v>0</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>2019</v>
@@ -641,13 +647,13 @@
     </row>
     <row r="20" spans="1:5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>0</v>
+        <v>12697000</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>2019</v>
@@ -658,10 +664,10 @@
     </row>
     <row r="21" spans="1:5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0</v>
@@ -675,10 +681,10 @@
     </row>
     <row r="22" spans="1:5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0</v>
@@ -692,10 +698,10 @@
     </row>
     <row r="23" spans="1:5" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>0</v>
@@ -709,10 +715,10 @@
     </row>
     <row r="24" spans="1:5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>0</v>
@@ -726,10 +732,10 @@
     </row>
     <row r="25" spans="1:5" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>0</v>
@@ -743,10 +749,10 @@
     </row>
     <row r="26" spans="1:5" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>0</v>
@@ -760,10 +766,10 @@
     </row>
     <row r="27" spans="1:5" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>0</v>
@@ -777,10 +783,10 @@
     </row>
     <row r="28" spans="1:5" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>0</v>
@@ -794,10 +800,10 @@
     </row>
     <row r="29" spans="1:5" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>0</v>
@@ -811,10 +817,10 @@
     </row>
     <row r="30" spans="1:5" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>0</v>
@@ -828,10 +834,10 @@
     </row>
     <row r="31" spans="1:5" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B31" s="1" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>0</v>
@@ -845,10 +851,10 @@
     </row>
     <row r="32" spans="1:5" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B32" s="1" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>0</v>
@@ -862,10 +868,10 @@
     </row>
     <row r="33" spans="1:5" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B33" s="1" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>0</v>
@@ -879,10 +885,10 @@
     </row>
     <row r="34" spans="1:5" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B34" s="1" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>0</v>
@@ -896,10 +902,10 @@
     </row>
     <row r="35" spans="1:5" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B35" s="1" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>0</v>
@@ -913,10 +919,10 @@
     </row>
     <row r="36" spans="1:5" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B36" s="1" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>0</v>
@@ -930,10 +936,10 @@
     </row>
     <row r="37" spans="1:5" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B37" s="1" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>0</v>
@@ -947,10 +953,10 @@
     </row>
     <row r="38" spans="1:5" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>0</v>
@@ -964,10 +970,10 @@
     </row>
     <row r="39" spans="1:5" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B39" s="1" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>0</v>
@@ -981,10 +987,10 @@
     </row>
     <row r="40" spans="1:5" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B40" s="1" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>0</v>
@@ -998,10 +1004,10 @@
     </row>
     <row r="41" spans="1:5" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B41" s="1" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>0</v>
@@ -1015,10 +1021,10 @@
     </row>
     <row r="42" spans="1:5" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B42" s="1" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>0</v>
@@ -1032,10 +1038,10 @@
     </row>
     <row r="43" spans="1:5" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B43" s="1" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>0</v>
@@ -1049,10 +1055,10 @@
     </row>
     <row r="44" spans="1:5" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B44" s="1" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>0</v>
@@ -1066,10 +1072,10 @@
     </row>
     <row r="45" spans="1:5" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B45" s="1" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>0</v>
@@ -1083,10 +1089,10 @@
     </row>
     <row r="46" spans="1:5" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B46" s="1" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>0</v>
@@ -1100,10 +1106,10 @@
     </row>
     <row r="47" spans="1:5" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B47" s="1" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>0</v>
@@ -1117,10 +1123,10 @@
     </row>
     <row r="48" spans="1:5" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B48" s="1" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>0</v>
@@ -1134,10 +1140,10 @@
     </row>
     <row r="49" spans="1:5" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B49" s="1" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>0</v>
@@ -1151,10 +1157,10 @@
     </row>
     <row r="50" spans="1:5" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B50" s="1" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>0</v>
@@ -1168,10 +1174,10 @@
     </row>
     <row r="51" spans="1:5" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B51" s="1" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>0</v>
@@ -1185,10 +1191,10 @@
     </row>
     <row r="52" spans="1:5" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B52" s="1" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>0</v>
@@ -1202,10 +1208,10 @@
     </row>
     <row r="53" spans="1:5" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B53" s="1" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>0</v>
@@ -1219,10 +1225,10 @@
     </row>
     <row r="54" spans="1:5" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B54" s="1" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>0</v>
@@ -1236,10 +1242,10 @@
     </row>
     <row r="55" spans="1:5" customHeight="1">
       <c r="A55" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B55" s="1" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>0</v>
@@ -1253,10 +1259,10 @@
     </row>
     <row r="56" spans="1:5" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B56" s="1" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>0</v>
@@ -1270,10 +1276,10 @@
     </row>
     <row r="57" spans="1:5" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B57" s="1" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>0</v>
@@ -1287,10 +1293,10 @@
     </row>
     <row r="58" spans="1:5" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B58" s="1" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>0</v>
@@ -1304,10 +1310,10 @@
     </row>
     <row r="59" spans="1:5" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B59" s="1" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>0</v>
@@ -1321,10 +1327,10 @@
     </row>
     <row r="60" spans="1:5" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B60" s="1" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>0</v>
@@ -1338,10 +1344,10 @@
     </row>
     <row r="61" spans="1:5" customHeight="1">
       <c r="A61" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B61" s="1" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C61" s="1" t="n">
         <v>0</v>
@@ -1355,10 +1361,10 @@
     </row>
     <row r="62" spans="1:5" customHeight="1">
       <c r="A62" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B62" s="1" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>0</v>
@@ -1372,10 +1378,10 @@
     </row>
     <row r="63" spans="1:5" customHeight="1">
       <c r="A63" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B63" s="1" t="n">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>0</v>
@@ -1389,10 +1395,10 @@
     </row>
     <row r="64" spans="1:5" customHeight="1">
       <c r="A64" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B64" s="1" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>0</v>
@@ -1406,10 +1412,10 @@
     </row>
     <row r="65" spans="1:5" customHeight="1">
       <c r="A65" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B65" s="1" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>0</v>
@@ -1423,10 +1429,10 @@
     </row>
     <row r="66" spans="1:5" customHeight="1">
       <c r="A66" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B66" s="1" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>0</v>
@@ -1440,10 +1446,10 @@
     </row>
     <row r="67" spans="1:5" customHeight="1">
       <c r="A67" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B67" s="1" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>0</v>
@@ -1457,10 +1463,10 @@
     </row>
     <row r="68" spans="1:5" customHeight="1">
       <c r="A68" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B68" s="1" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C68" s="1" t="n">
         <v>0</v>
@@ -1474,10 +1480,10 @@
     </row>
     <row r="69" spans="1:5" customHeight="1">
       <c r="A69" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B69" s="1" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C69" s="1" t="n">
         <v>0</v>
@@ -1491,10 +1497,10 @@
     </row>
     <row r="70" spans="1:5" customHeight="1">
       <c r="A70" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B70" s="1" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C70" s="1" t="n">
         <v>0</v>
@@ -1508,10 +1514,10 @@
     </row>
     <row r="71" spans="1:5" customHeight="1">
       <c r="A71" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B71" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C71" s="1" t="n">
         <v>0</v>
@@ -1525,10 +1531,10 @@
     </row>
     <row r="72" spans="1:5" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B72" s="1" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>0</v>
@@ -1542,10 +1548,10 @@
     </row>
     <row r="73" spans="1:5" customHeight="1">
       <c r="A73" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B73" s="1" t="n">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>0</v>
@@ -1559,10 +1565,10 @@
     </row>
     <row r="74" spans="1:5" customHeight="1">
       <c r="A74" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B74" s="1" t="n">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>0</v>
@@ -1576,10 +1582,10 @@
     </row>
     <row r="75" spans="1:5" customHeight="1">
       <c r="A75" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B75" s="1" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C75" s="1" t="n">
         <v>0</v>
@@ -1593,18 +1599,35 @@
     </row>
     <row r="76" spans="1:5" customHeight="1">
       <c r="A76" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B76" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="C76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D76" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" customHeight="1">
+      <c r="A77" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B77" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="C76" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D76" s="1" t="n">
-        <v>2019</v>
-      </c>
-      <c r="E76" s="1" t="s">
+      <c r="C77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>